<commit_message>
encountered strange bug in loading sets for variables not defined on all coordinates
</commit_message>
<xml_diff>
--- a/tests/models/integrated/4_full_scale_model/model_settings.xlsx
+++ b/tests/models/integrated/4_full_scale_model/model_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzorinaldi/Documents/GitHub/pyesm/tests/models/integrated/4_full_scale_model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729A502B-74F8-EB42-A8FB-20C8176C9403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8D2AB7-AA0C-2048-BAB1-57348B478196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="6220" windowWidth="30240" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9200" yWindow="-28800" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{E7BE83BA-6F55-CD4E-965C-CAB718F8F3E7}"/>
   </bookViews>
   <sheets>
     <sheet name="structure_sets" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="168">
   <si>
     <t>set_key</t>
   </si>
@@ -121,9 +121,6 @@
     <t>X_e</t>
   </si>
   <si>
-    <t>E_hist,ex</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -148,12 +145,6 @@
     <t>dim: cols, filters: {type_physical: [final]}</t>
   </si>
   <si>
-    <t>dim: intra, filters: {time_scope:[model]}</t>
-  </si>
-  <si>
-    <t>dim: intra, filters: {time_scope:[historical]}</t>
-  </si>
-  <si>
     <t>pe_type: [emissions by tech, emissions by prod, primary resources]</t>
   </si>
   <si>
@@ -181,9 +172,6 @@
     <t>E_hist_ex</t>
   </si>
   <si>
-    <t>Q_yy - mult(u_yy, tran(X_yy)) - mult(u_yh, tran(X_yh)) - mult(E_y, i_tf) == 0</t>
-  </si>
-  <si>
     <t>i_tf</t>
   </si>
   <si>
@@ -316,9 +304,6 @@
     <t>I_yy</t>
   </si>
   <si>
-    <t>identity_rcot</t>
-  </si>
-  <si>
     <t>I_hh</t>
   </si>
   <si>
@@ -367,9 +352,6 @@
     <t>Q_yh</t>
   </si>
   <si>
-    <t>Q_y_blend</t>
-  </si>
-  <si>
     <t>Q_h</t>
   </si>
   <si>
@@ -439,9 +421,6 @@
     <t>M_h</t>
   </si>
   <si>
-    <t>dim: intra, filters: {region: [row]}</t>
-  </si>
-  <si>
     <t>r_v</t>
   </si>
   <si>
@@ -460,9 +439,6 @@
     <t>r_v_env_p</t>
   </si>
   <si>
-    <t>dim: intra, filters:{pe_type:[emissions by prod]}</t>
-  </si>
-  <si>
     <t>r_v_b_out</t>
   </si>
   <si>
@@ -511,9 +487,6 @@
     <t>R_ve</t>
   </si>
   <si>
-    <t>RR_vu,C</t>
-  </si>
-  <si>
     <t>R_vu_C</t>
   </si>
   <si>
@@ -553,7 +526,22 @@
     <t>sectors, technologies</t>
   </si>
   <si>
-    <t>aggregation</t>
+    <t>Q_y_b</t>
+  </si>
+  <si>
+    <t>filters: {time_scope:[model]}</t>
+  </si>
+  <si>
+    <t>filters: {time_scope:[historical]}</t>
+  </si>
+  <si>
+    <t>filters: {region: [row]}</t>
+  </si>
+  <si>
+    <t>filters:{pe_type:[emissions by prod]}</t>
+  </si>
+  <si>
+    <t>RR_vu_C</t>
   </si>
 </sst>
 </file>
@@ -660,14 +648,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF0EFEB1-6ECC-43D2-AB72-C998AF198F27}" name="Table1" displayName="Table1" ref="A1:F7" totalsRowShown="0">
-  <autoFilter ref="A1:F7" xr:uid="{BF0EFEB1-6ECC-43D2-AB72-C998AF198F27}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF0EFEB1-6ECC-43D2-AB72-C998AF198F27}" name="Table1" displayName="Table1" ref="A1:E7" totalsRowShown="0">
+  <autoFilter ref="A1:E7" xr:uid="{BF0EFEB1-6ECC-43D2-AB72-C998AF198F27}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B25B1879-C5E9-4EB5-B028-F8512D272279}" name="set_key"/>
     <tableColumn id="9" xr3:uid="{DF8CC285-45E4-43D5-B8D8-803C745D6940}" name="description"/>
     <tableColumn id="4" xr3:uid="{A3D9FB3A-774D-46EA-8E98-EFD15E392CBD}" name="split_problem"/>
     <tableColumn id="2" xr3:uid="{63BC0DE3-0E2B-46D5-92FB-25DE1E0A2CA9}" name="copy_from"/>
-    <tableColumn id="3" xr3:uid="{2A37340B-18B6-3046-8916-AFA39BFCF149}" name="aggregation"/>
     <tableColumn id="8" xr3:uid="{AD5E32F7-2499-45CB-8B2A-F64E57F8E7E0}" name="filters"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -697,8 +684,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9E7FEE58-959B-4A76-BD2C-C7A4A140E173}" name="Table4" displayName="Table4" ref="A1:C5" totalsRowShown="0">
-  <autoFilter ref="A1:C5" xr:uid="{9E7FEE58-959B-4A76-BD2C-C7A4A140E173}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9E7FEE58-959B-4A76-BD2C-C7A4A140E173}" name="Table4" displayName="Table4" ref="A1:C19" totalsRowShown="0">
+  <autoFilter ref="A1:C19" xr:uid="{9E7FEE58-959B-4A76-BD2C-C7A4A140E173}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{339B6BC6-DC77-44F3-BC7D-5887B7C1C68A}" name="problem_key" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{7D3A5DDD-E4D2-4BFD-8F61-20DAAF76C565}" name="objective"/>
@@ -971,22 +958,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView zoomScale="244" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="33.83203125" customWidth="1"/>
-    <col min="3" max="5" width="15.1640625" customWidth="1"/>
-    <col min="6" max="6" width="103.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.5" customWidth="1"/>
+    <col min="3" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="103.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1000,13 +987,10 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1015,23 +999,22 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" t="s">
+      <c r="E2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1039,13 +1022,10 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1053,26 +1033,26 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="F7" t="s">
-        <v>38</v>
+      <c r="E7" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1088,11 +1068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F872E8C-C62E-4F3F-A20F-41906D0144C1}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1155,387 +1132,378 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s">
         <v>71</v>
       </c>
-      <c r="B3" t="s">
+      <c r="H3" t="s">
         <v>72</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H3" t="s">
-        <v>76</v>
-      </c>
       <c r="I3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" t="s">
         <v>73</v>
       </c>
-      <c r="F4" t="s">
-        <v>77</v>
-      </c>
       <c r="H4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="F12" t="s">
-        <v>91</v>
-      </c>
-      <c r="G12" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="F13" t="s">
-        <v>93</v>
-      </c>
-      <c r="G13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>161</v>
+      </c>
+      <c r="F14" t="s">
         <v>89</v>
       </c>
-      <c r="B14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s">
-        <v>170</v>
-      </c>
-      <c r="F14" t="s">
-        <v>94</v>
-      </c>
-      <c r="G14" t="s">
-        <v>92</v>
-      </c>
       <c r="H14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J14" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B15" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F15" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H15" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F16" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H16" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F17" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H17" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
@@ -1544,7 +1512,7 @@
         <v>18</v>
       </c>
       <c r="F18" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1552,22 +1520,22 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F19" t="s">
         <v>25</v>
       </c>
       <c r="I19" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" t="s">
         <v>34</v>
-      </c>
-      <c r="J19" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1575,22 +1543,22 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F20" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I20" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1598,30 +1566,30 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F21" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="I21" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
@@ -1630,867 +1598,867 @@
         <v>31</v>
       </c>
       <c r="F22" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" t="s">
+        <v>33</v>
+      </c>
+      <c r="J22" t="s">
+        <v>34</v>
+      </c>
+      <c r="L22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" t="s">
         <v>26</v>
       </c>
-      <c r="B23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" t="s">
-        <v>31</v>
-      </c>
-      <c r="F23" t="s">
-        <v>44</v>
-      </c>
       <c r="J23" t="s">
-        <v>35</v>
-      </c>
-      <c r="L23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>27</v>
+      <c r="A24" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" t="s">
         <v>41</v>
       </c>
-      <c r="C24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" t="s">
-        <v>46</v>
-      </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>34</v>
       </c>
-      <c r="J24" t="s">
-        <v>35</v>
-      </c>
       <c r="L24" t="s">
-        <v>37</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" t="s">
         <v>28</v>
       </c>
-      <c r="B25" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" t="s">
-        <v>29</v>
-      </c>
       <c r="E25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J25" t="s">
         <v>34</v>
-      </c>
-      <c r="J25" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s">
         <v>28</v>
       </c>
-      <c r="B26" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" t="s">
-        <v>29</v>
-      </c>
       <c r="E26" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" t="s">
         <v>32</v>
       </c>
-      <c r="F26" t="s">
+      <c r="I26" t="s">
         <v>33</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>34</v>
       </c>
-      <c r="J26" t="s">
-        <v>35</v>
-      </c>
       <c r="L26" t="s">
-        <v>37</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
         <v>28</v>
       </c>
-      <c r="B27" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" t="s">
-        <v>29</v>
-      </c>
       <c r="E27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F27" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I27" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L27" t="s">
-        <v>36</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
         <v>28</v>
       </c>
-      <c r="B28" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" t="s">
-        <v>29</v>
-      </c>
       <c r="E28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F28" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I28" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L28" t="s">
-        <v>36</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C29" t="s">
         <v>7</v>
       </c>
       <c r="E29" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" t="s">
+        <v>100</v>
+      </c>
+      <c r="I29" t="s">
+        <v>80</v>
+      </c>
+      <c r="K29" t="s">
         <v>107</v>
-      </c>
-      <c r="F29" t="s">
-        <v>105</v>
-      </c>
-      <c r="I29" t="s">
-        <v>84</v>
-      </c>
-      <c r="K29" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30" t="s">
+        <v>49</v>
+      </c>
+      <c r="I30" t="s">
         <v>53</v>
-      </c>
-      <c r="B30" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" t="s">
-        <v>55</v>
-      </c>
-      <c r="E30" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30" t="s">
-        <v>53</v>
-      </c>
-      <c r="I30" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31" t="s">
         <v>54</v>
       </c>
-      <c r="C31" t="s">
+      <c r="I31" t="s">
         <v>55</v>
-      </c>
-      <c r="E31" t="s">
-        <v>56</v>
-      </c>
-      <c r="F31" t="s">
-        <v>58</v>
-      </c>
-      <c r="I31" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E32" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F32" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="I32" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E33" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F33" t="s">
-        <v>109</v>
+        <v>162</v>
       </c>
       <c r="I33" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E34" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F34" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="I34" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="K34" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F35" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="J35" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" t="s">
+        <v>59</v>
+      </c>
+      <c r="J36" t="s">
         <v>60</v>
-      </c>
-      <c r="B36" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" t="s">
-        <v>55</v>
-      </c>
-      <c r="E36" t="s">
-        <v>31</v>
-      </c>
-      <c r="F36" t="s">
-        <v>63</v>
-      </c>
-      <c r="J36" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" t="s">
+        <v>51</v>
+      </c>
+      <c r="E37" t="s">
+        <v>30</v>
+      </c>
+      <c r="F37" t="s">
         <v>61</v>
       </c>
-      <c r="C37" t="s">
-        <v>55</v>
-      </c>
-      <c r="E37" t="s">
-        <v>31</v>
-      </c>
-      <c r="F37" t="s">
-        <v>65</v>
-      </c>
       <c r="J37" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F38" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="J38" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B39" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E39" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F39" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="J39" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="K39" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B40" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E40" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F40" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H40" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I40" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B41" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F41" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="I41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J41" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B42" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E42" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F42" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="H42" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I42" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B43" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E43" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F43" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H43" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I43" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B44" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C44" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E44" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F44" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="H44" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
       <c r="I44" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="K44" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B45" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C45" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E45" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F45" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="I45" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M45" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B46" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C46" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E46" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F46" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="I46" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M46" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B47" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C47" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E47" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F47" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="I47" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="M47" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B48" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48" t="s">
+        <v>129</v>
+      </c>
+      <c r="E48" t="s">
+        <v>130</v>
+      </c>
+      <c r="F48" t="s">
         <v>134</v>
       </c>
-      <c r="B48" t="s">
+      <c r="I48" t="s">
         <v>135</v>
       </c>
-      <c r="C48" t="s">
-        <v>136</v>
-      </c>
-      <c r="E48" t="s">
-        <v>137</v>
-      </c>
-      <c r="F48" t="s">
-        <v>142</v>
-      </c>
-      <c r="I48" t="s">
-        <v>143</v>
-      </c>
       <c r="M48" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B49" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E49" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F49" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="J49" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="M49" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B50" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
       </c>
       <c r="E50" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="F50" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="I50" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J50" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="M50" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B51" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
       </c>
       <c r="E51" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="F51" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="I51" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J51" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="M51" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B52" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E52" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="F52" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="I52" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J52" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="M52" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B53" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E53" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="F53" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="I53" t="s">
+        <v>33</v>
+      </c>
+      <c r="J53" t="s">
         <v>34</v>
       </c>
-      <c r="J53" t="s">
-        <v>35</v>
-      </c>
       <c r="M53" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="B54" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E54" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="F54" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="I54" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J54" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="M54" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B55" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C55" t="s">
         <v>7</v>
       </c>
       <c r="E55" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F55" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="J55" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="M55" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B56" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C56" t="s">
         <v>7</v>
       </c>
       <c r="E56" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F56" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="J56" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M56" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B57" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E57" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F57" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="J57" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="M57" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B58" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C58" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E58" t="s">
         <v>17</v>
       </c>
       <c r="F58" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G58" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J58" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B59" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E59" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F59" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="J59" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M59" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2503,17 +2471,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB4DB9B-67B8-45E9-9CD6-D02B1BE46AE7}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" customWidth="1"/>
-    <col min="3" max="3" width="87.83203125" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="80.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2532,7 +2500,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2540,15 +2508,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2560,26 +2520,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c319d79e-6821-4c2a-8db8-88a02643e5e3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="aa97a2c6-5066-49ad-90c0-e23f9da31bb2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D81D9CE2A426814A9054AC6C4C722ED5" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="64dce91d1c025dd40a65521324b61665">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="aa97a2c6-5066-49ad-90c0-e23f9da31bb2" xmlns:ns3="c319d79e-6821-4c2a-8db8-88a02643e5e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0b6c53cd2d86a7b8a56cde2aeea85a90" ns2:_="" ns3:_="">
     <xsd:import namespace="aa97a2c6-5066-49ad-90c0-e23f9da31bb2"/>
@@ -2780,7 +2720,46 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c319d79e-6821-4c2a-8db8-88a02643e5e3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="aa97a2c6-5066-49ad-90c0-e23f9da31bb2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2294B864-0C2E-4EE7-BC4B-97F56F3E1E6F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="aa97a2c6-5066-49ad-90c0-e23f9da31bb2"/>
+    <ds:schemaRef ds:uri="c319d79e-6821-4c2a-8db8-88a02643e5e3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A76C88C-3CD9-4DB8-BDE8-13FD5F7691CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2797,29 +2776,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F8ED70-8537-426E-A479-D2342A5FB5EB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2294B864-0C2E-4EE7-BC4B-97F56F3E1E6F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="aa97a2c6-5066-49ad-90c0-e23f9da31bb2"/>
-    <ds:schemaRef ds:uri="c319d79e-6821-4c2a-8db8-88a02643e5e3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
"all sets and variables validated"
</commit_message>
<xml_diff>
--- a/tests/models/integrated/4_full_scale_model/model_settings.xlsx
+++ b/tests/models/integrated/4_full_scale_model/model_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzorinaldi/Documents/GitHub/pyesm/tests/models/integrated/4_full_scale_model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baioc\Documents\GitHub\pyesm\tests\models\integrated\4_full_scale_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2CDE1D-3E9C-2341-A258-A64167FC9FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D257BC3-63F1-4DCF-89E1-ACA897C3E29A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9240" yWindow="-28800" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{E7BE83BA-6F55-CD4E-965C-CAB718F8F3E7}"/>
+    <workbookView xWindow="29970" yWindow="1170" windowWidth="23010" windowHeight="13650" activeTab="1" xr2:uid="{E7BE83BA-6F55-CD4E-965C-CAB718F8F3E7}"/>
   </bookViews>
   <sheets>
     <sheet name="structure_sets" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="168">
   <si>
     <t>set_key</t>
   </si>
@@ -187,9 +187,6 @@
     <t>total demand by technology by year</t>
   </si>
   <si>
-    <t>0: endogenous, 1: exogenous</t>
-  </si>
-  <si>
     <t>products, years</t>
   </si>
   <si>
@@ -415,9 +412,6 @@
     <t>environmental transactions - by product</t>
   </si>
   <si>
-    <t>0: exogenous, 1: endogenous</t>
-  </si>
-  <si>
     <t>products_env, products, years</t>
   </si>
   <si>
@@ -538,13 +532,16 @@
     <t>dim: intra, filters: {time_scope:[model]}</t>
   </si>
   <si>
-    <t>E == mult(e, tran(X_e_mod))</t>
-  </si>
-  <si>
     <t>pl</t>
   </si>
   <si>
     <t>periods length</t>
+  </si>
+  <si>
+    <t>1: endogenous, 2: exogenous</t>
+  </si>
+  <si>
+    <t>1: exogenous, 2: endogenous</t>
   </si>
 </sst>
 </file>
@@ -687,8 +684,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9E7FEE58-959B-4A76-BD2C-C7A4A140E173}" name="Table4" displayName="Table4" ref="A1:C19" totalsRowShown="0">
-  <autoFilter ref="A1:C19" xr:uid="{9E7FEE58-959B-4A76-BD2C-C7A4A140E173}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9E7FEE58-959B-4A76-BD2C-C7A4A140E173}" name="Table4" displayName="Table4" ref="A1:C18" totalsRowShown="0">
+  <autoFilter ref="A1:C18" xr:uid="{9E7FEE58-959B-4A76-BD2C-C7A4A140E173}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{339B6BC6-DC77-44F3-BC7D-5887B7C1C68A}" name="problem_key" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{7D3A5DDD-E4D2-4BFD-8F61-20DAAF76C565}" name="objective"/>
@@ -967,16 +964,16 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="33.83203125" customWidth="1"/>
-    <col min="3" max="4" width="15.1640625" customWidth="1"/>
-    <col min="5" max="5" width="103.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="103.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -993,7 +990,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1006,7 +1003,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1014,10 +1011,10 @@
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1028,7 +1025,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1036,7 +1033,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1047,7 +1044,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1071,28 +1068,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F872E8C-C62E-4F3F-A20F-41906D0144C1}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="117" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45:C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="8" width="52" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="58" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="51.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="51.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1133,104 +1130,104 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
         <v>65</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" t="s">
         <v>67</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
         <v>65</v>
       </c>
-      <c r="H2" t="s">
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" t="s">
         <v>68</v>
       </c>
-      <c r="I2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="H3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
         <v>65</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
         <v>66</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="F4" t="s">
         <v>70</v>
       </c>
-      <c r="I3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="H4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
         <v>65</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
         <v>66</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" t="s">
-        <v>71</v>
-      </c>
-      <c r="H4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="F5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>74</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>75</v>
       </c>
-      <c r="I5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
         <v>61</v>
-      </c>
-      <c r="B6" t="s">
-        <v>62</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -1239,21 +1236,21 @@
         <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I6" t="s">
         <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
         <v>61</v>
-      </c>
-      <c r="B7" t="s">
-        <v>62</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -1262,21 +1259,21 @@
         <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I7" t="s">
         <v>46</v>
       </c>
       <c r="J7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
         <v>61</v>
-      </c>
-      <c r="B8" t="s">
-        <v>62</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -1285,21 +1282,21 @@
         <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I8" t="s">
         <v>46</v>
       </c>
       <c r="J8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>61</v>
-      </c>
-      <c r="B9" t="s">
-        <v>62</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -1308,21 +1305,21 @@
         <v>29</v>
       </c>
       <c r="F9" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" t="s">
         <v>77</v>
       </c>
-      <c r="I9" t="s">
-        <v>78</v>
-      </c>
       <c r="J9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
         <v>61</v>
-      </c>
-      <c r="B10" t="s">
-        <v>62</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -1331,21 +1328,21 @@
         <v>29</v>
       </c>
       <c r="F10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>61</v>
-      </c>
-      <c r="B11" t="s">
-        <v>62</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -1354,159 +1351,159 @@
         <v>29</v>
       </c>
       <c r="F11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I11" t="s">
         <v>80</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>81</v>
       </c>
-      <c r="J11" t="s">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>83</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>155</v>
+      </c>
+      <c r="F12" t="s">
         <v>84</v>
       </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" t="s">
-        <v>157</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>155</v>
+      </c>
+      <c r="F13" t="s">
         <v>85</v>
       </c>
-      <c r="H12" t="s">
-        <v>70</v>
-      </c>
-      <c r="J12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="H13" t="s">
+        <v>71</v>
+      </c>
+      <c r="J13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" t="s">
         <v>83</v>
       </c>
-      <c r="B13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>157</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>155</v>
+      </c>
+      <c r="F14" t="s">
         <v>86</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H14" t="s">
+        <v>74</v>
+      </c>
+      <c r="J14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" t="s">
+        <v>87</v>
+      </c>
+      <c r="H15" t="s">
+        <v>89</v>
+      </c>
+      <c r="I15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" t="s">
+        <v>89</v>
+      </c>
+      <c r="I17" t="s">
         <v>72</v>
       </c>
-      <c r="J13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>83</v>
-      </c>
-      <c r="B14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s">
-        <v>157</v>
-      </c>
-      <c r="F14" t="s">
-        <v>87</v>
-      </c>
-      <c r="H14" t="s">
-        <v>75</v>
-      </c>
-      <c r="J14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" t="s">
-        <v>88</v>
-      </c>
-      <c r="H15" t="s">
-        <v>90</v>
-      </c>
-      <c r="I15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" t="s">
-        <v>91</v>
-      </c>
-      <c r="H16" t="s">
-        <v>90</v>
-      </c>
-      <c r="I16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" t="s">
-        <v>92</v>
-      </c>
-      <c r="H17" t="s">
-        <v>90</v>
-      </c>
-      <c r="I17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B18" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
@@ -1515,10 +1512,10 @@
         <v>18</v>
       </c>
       <c r="F18" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1541,7 +1538,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1555,7 +1552,7 @@
         <v>29</v>
       </c>
       <c r="F20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I20" t="s">
         <v>46</v>
@@ -1564,7 +1561,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1578,16 +1575,16 @@
         <v>29</v>
       </c>
       <c r="F21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J21" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1610,10 +1607,10 @@
         <v>34</v>
       </c>
       <c r="L22" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
@@ -1633,7 +1630,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>26</v>
       </c>
@@ -1653,12 +1650,12 @@
         <v>34</v>
       </c>
       <c r="L24" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B25" t="s">
         <v>39</v>
@@ -1679,9 +1676,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B26" t="s">
         <v>39</v>
@@ -1702,12 +1699,12 @@
         <v>34</v>
       </c>
       <c r="L26" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B27" t="s">
         <v>39</v>
@@ -1728,12 +1725,12 @@
         <v>34</v>
       </c>
       <c r="L27" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B28" t="s">
         <v>39</v>
@@ -1745,42 +1742,42 @@
         <v>31</v>
       </c>
       <c r="F28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J28" t="s">
         <v>34</v>
       </c>
       <c r="L28" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" t="s">
         <v>96</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
         <v>97</v>
       </c>
-      <c r="C29" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" t="s">
-        <v>98</v>
-      </c>
       <c r="F29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K29" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -1788,19 +1785,19 @@
         <v>48</v>
       </c>
       <c r="C30" t="s">
+        <v>166</v>
+      </c>
+      <c r="E30" t="s">
         <v>49</v>
-      </c>
-      <c r="E30" t="s">
-        <v>50</v>
       </c>
       <c r="F30" t="s">
         <v>47</v>
       </c>
       <c r="I30" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -1808,19 +1805,19 @@
         <v>48</v>
       </c>
       <c r="C31" t="s">
+        <v>166</v>
+      </c>
+      <c r="E31" t="s">
         <v>49</v>
       </c>
-      <c r="E31" t="s">
-        <v>50</v>
-      </c>
       <c r="F31" t="s">
+        <v>51</v>
+      </c>
+      <c r="I31" t="s">
         <v>52</v>
       </c>
-      <c r="I31" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -1828,19 +1825,19 @@
         <v>48</v>
       </c>
       <c r="C32" t="s">
+        <v>166</v>
+      </c>
+      <c r="E32" t="s">
         <v>49</v>
       </c>
-      <c r="E32" t="s">
-        <v>50</v>
-      </c>
       <c r="F32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -1848,173 +1845,173 @@
         <v>48</v>
       </c>
       <c r="C33" t="s">
+        <v>166</v>
+      </c>
+      <c r="E33" t="s">
         <v>49</v>
       </c>
-      <c r="E33" t="s">
-        <v>50</v>
-      </c>
       <c r="F33" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I33" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" t="s">
         <v>100</v>
-      </c>
-      <c r="B34" t="s">
-        <v>101</v>
       </c>
       <c r="C34" t="s">
         <v>28</v>
       </c>
       <c r="E34" t="s">
+        <v>101</v>
+      </c>
+      <c r="F34" t="s">
+        <v>99</v>
+      </c>
+      <c r="I34" t="s">
+        <v>72</v>
+      </c>
+      <c r="K34" t="s">
         <v>102</v>
       </c>
-      <c r="F34" t="s">
-        <v>100</v>
-      </c>
-      <c r="I34" t="s">
-        <v>73</v>
-      </c>
-      <c r="K34" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" t="s">
         <v>54</v>
       </c>
-      <c r="B35" t="s">
-        <v>55</v>
-      </c>
       <c r="C35" t="s">
-        <v>49</v>
+        <v>166</v>
       </c>
       <c r="E35" t="s">
         <v>30</v>
       </c>
       <c r="F35" t="s">
+        <v>53</v>
+      </c>
+      <c r="J35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" t="s">
         <v>54</v>
       </c>
-      <c r="J35" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>54</v>
-      </c>
-      <c r="B36" t="s">
-        <v>55</v>
-      </c>
       <c r="C36" t="s">
-        <v>49</v>
+        <v>166</v>
       </c>
       <c r="E36" t="s">
         <v>30</v>
       </c>
       <c r="F36" t="s">
+        <v>56</v>
+      </c>
+      <c r="J36" t="s">
         <v>57</v>
       </c>
-      <c r="J36" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" t="s">
         <v>54</v>
       </c>
-      <c r="B37" t="s">
-        <v>55</v>
-      </c>
       <c r="C37" t="s">
-        <v>49</v>
+        <v>166</v>
       </c>
       <c r="E37" t="s">
         <v>30</v>
       </c>
       <c r="F37" t="s">
+        <v>58</v>
+      </c>
+      <c r="J37" t="s">
         <v>59</v>
       </c>
-      <c r="J37" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" t="s">
         <v>54</v>
       </c>
-      <c r="B38" t="s">
-        <v>55</v>
-      </c>
       <c r="C38" t="s">
-        <v>49</v>
+        <v>166</v>
       </c>
       <c r="E38" t="s">
         <v>30</v>
       </c>
       <c r="F38" t="s">
+        <v>103</v>
+      </c>
+      <c r="J38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>104</v>
       </c>
-      <c r="J38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="B39" t="s">
         <v>105</v>
-      </c>
-      <c r="B39" t="s">
-        <v>106</v>
       </c>
       <c r="C39" t="s">
         <v>28</v>
       </c>
       <c r="E39" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39" t="s">
+        <v>104</v>
+      </c>
+      <c r="J39" t="s">
+        <v>59</v>
+      </c>
+      <c r="K39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>107</v>
       </c>
-      <c r="F39" t="s">
-        <v>105</v>
-      </c>
-      <c r="J39" t="s">
-        <v>60</v>
-      </c>
-      <c r="K39" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
         <v>108</v>
-      </c>
-      <c r="B40" t="s">
-        <v>109</v>
       </c>
       <c r="C40" t="s">
         <v>28</v>
       </c>
       <c r="E40" t="s">
+        <v>109</v>
+      </c>
+      <c r="F40" t="s">
         <v>110</v>
       </c>
-      <c r="F40" t="s">
+      <c r="H40" t="s">
+        <v>67</v>
+      </c>
+      <c r="I40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>111</v>
       </c>
-      <c r="H40" t="s">
-        <v>68</v>
-      </c>
-      <c r="I40" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
         <v>112</v>
-      </c>
-      <c r="B41" t="s">
-        <v>113</v>
       </c>
       <c r="C41" t="s">
         <v>28</v>
@@ -2023,295 +2020,295 @@
         <v>31</v>
       </c>
       <c r="F41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I41" t="s">
         <v>33</v>
       </c>
       <c r="J41" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" t="s">
         <v>115</v>
-      </c>
-      <c r="B42" t="s">
-        <v>116</v>
       </c>
       <c r="C42" t="s">
         <v>28</v>
       </c>
       <c r="E42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I42" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>114</v>
+      </c>
+      <c r="B43" t="s">
         <v>115</v>
-      </c>
-      <c r="B43" t="s">
-        <v>116</v>
       </c>
       <c r="C43" t="s">
         <v>28</v>
       </c>
       <c r="E43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F43" t="s">
+        <v>117</v>
+      </c>
+      <c r="H43" t="s">
+        <v>89</v>
+      </c>
+      <c r="I43" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>118</v>
       </c>
-      <c r="H43" t="s">
-        <v>90</v>
-      </c>
-      <c r="I43" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="B44" t="s">
         <v>119</v>
-      </c>
-      <c r="B44" t="s">
-        <v>120</v>
       </c>
       <c r="C44" t="s">
         <v>28</v>
       </c>
       <c r="E44" t="s">
+        <v>120</v>
+      </c>
+      <c r="F44" t="s">
         <v>121</v>
       </c>
-      <c r="F44" t="s">
+      <c r="H44" t="s">
+        <v>159</v>
+      </c>
+      <c r="I44" t="s">
+        <v>72</v>
+      </c>
+      <c r="K44" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>122</v>
       </c>
-      <c r="H44" t="s">
-        <v>161</v>
-      </c>
-      <c r="I44" t="s">
-        <v>73</v>
-      </c>
-      <c r="K44" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="B45" t="s">
         <v>123</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
+        <v>167</v>
+      </c>
+      <c r="E45" t="s">
         <v>124</v>
       </c>
-      <c r="C45" t="s">
+      <c r="F45" t="s">
+        <v>122</v>
+      </c>
+      <c r="I45" t="s">
+        <v>50</v>
+      </c>
+      <c r="M45" t="s">
         <v>125</v>
       </c>
-      <c r="E45" t="s">
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>122</v>
+      </c>
+      <c r="B46" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46" t="s">
+        <v>167</v>
+      </c>
+      <c r="E46" t="s">
+        <v>124</v>
+      </c>
+      <c r="F46" t="s">
         <v>126</v>
       </c>
-      <c r="F45" t="s">
+      <c r="I46" t="s">
+        <v>50</v>
+      </c>
+      <c r="M46" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B47" t="s">
         <v>123</v>
       </c>
-      <c r="I45" t="s">
-        <v>51</v>
-      </c>
-      <c r="M45" t="s">
+      <c r="C47" t="s">
+        <v>167</v>
+      </c>
+      <c r="E47" t="s">
+        <v>124</v>
+      </c>
+      <c r="F47" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="I47" t="s">
+        <v>75</v>
+      </c>
+      <c r="M47" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B48" t="s">
         <v>123</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C48" t="s">
+        <v>167</v>
+      </c>
+      <c r="E48" t="s">
         <v>124</v>
       </c>
-      <c r="C46" t="s">
+      <c r="F48" t="s">
+        <v>128</v>
+      </c>
+      <c r="I48" t="s">
+        <v>129</v>
+      </c>
+      <c r="M48" t="s">
         <v>125</v>
       </c>
-      <c r="E46" t="s">
-        <v>126</v>
-      </c>
-      <c r="F46" t="s">
-        <v>128</v>
-      </c>
-      <c r="I46" t="s">
-        <v>51</v>
-      </c>
-      <c r="M46" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B47" t="s">
-        <v>124</v>
-      </c>
-      <c r="C47" t="s">
-        <v>125</v>
-      </c>
-      <c r="E47" t="s">
-        <v>126</v>
-      </c>
-      <c r="F47" t="s">
-        <v>129</v>
-      </c>
-      <c r="I47" t="s">
-        <v>76</v>
-      </c>
-      <c r="M47" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B48" t="s">
-        <v>124</v>
-      </c>
-      <c r="C48" t="s">
-        <v>125</v>
-      </c>
-      <c r="E48" t="s">
-        <v>126</v>
-      </c>
-      <c r="F48" t="s">
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="I48" t="s">
+      <c r="B49" t="s">
         <v>131</v>
       </c>
-      <c r="M48" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
+      <c r="C49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" t="s">
         <v>132</v>
       </c>
-      <c r="B49" t="s">
+      <c r="F49" t="s">
+        <v>130</v>
+      </c>
+      <c r="J49" t="s">
+        <v>55</v>
+      </c>
+      <c r="M49" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="B50" t="s">
         <v>134</v>
       </c>
-      <c r="F49" t="s">
-        <v>132</v>
-      </c>
-      <c r="J49" t="s">
-        <v>56</v>
-      </c>
-      <c r="M49" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" t="s">
         <v>135</v>
       </c>
-      <c r="B50" t="s">
-        <v>136</v>
-      </c>
-      <c r="C50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50" t="s">
-        <v>137</v>
-      </c>
       <c r="F50" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I50" t="s">
         <v>33</v>
       </c>
       <c r="J50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M50" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
       </c>
       <c r="E51" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F51" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I51" t="s">
         <v>33</v>
       </c>
       <c r="J51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M51" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B52" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E52" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F52" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I52" t="s">
         <v>33</v>
       </c>
       <c r="J52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M52" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B53" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E53" t="s">
+        <v>140</v>
+      </c>
+      <c r="F53" t="s">
         <v>142</v>
-      </c>
-      <c r="F53" t="s">
-        <v>144</v>
       </c>
       <c r="I53" t="s">
         <v>33</v>
@@ -2320,110 +2317,110 @@
         <v>34</v>
       </c>
       <c r="M53" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B54" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F54" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I54" t="s">
         <v>33</v>
       </c>
       <c r="J54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M54" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>144</v>
+      </c>
+      <c r="B55" t="s">
+        <v>145</v>
+      </c>
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" t="s">
+        <v>132</v>
+      </c>
+      <c r="F55" t="s">
         <v>146</v>
       </c>
-      <c r="B55" t="s">
+      <c r="J55" t="s">
+        <v>55</v>
+      </c>
+      <c r="M55" t="s">
         <v>147</v>
       </c>
-      <c r="C55" t="s">
-        <v>7</v>
-      </c>
-      <c r="E55" t="s">
-        <v>134</v>
-      </c>
-      <c r="F55" t="s">
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>144</v>
+      </c>
+      <c r="B56" t="s">
+        <v>145</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" t="s">
+        <v>132</v>
+      </c>
+      <c r="F56" t="s">
         <v>148</v>
-      </c>
-      <c r="J55" t="s">
-        <v>56</v>
-      </c>
-      <c r="M55" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>146</v>
-      </c>
-      <c r="B56" t="s">
-        <v>147</v>
-      </c>
-      <c r="C56" t="s">
-        <v>7</v>
-      </c>
-      <c r="E56" t="s">
-        <v>134</v>
-      </c>
-      <c r="F56" t="s">
-        <v>150</v>
       </c>
       <c r="J56" t="s">
         <v>34</v>
       </c>
       <c r="M56" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
-        <v>151</v>
-      </c>
       <c r="B57" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E57" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F57" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M57" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>42</v>
       </c>
       <c r="B58" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C58" t="s">
         <v>43</v>
@@ -2441,27 +2438,27 @@
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B59" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E59" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F59" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J59" t="s">
         <v>34</v>
       </c>
       <c r="M59" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2474,20 +2471,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB4DB9B-67B8-45E9-9CD6-D02B1BE46AE7}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="80.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2496,14 +2493,6 @@
       </c>
       <c r="C1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2515,6 +2504,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c319d79e-6821-4c2a-8db8-88a02643e5e3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="aa97a2c6-5066-49ad-90c0-e23f9da31bb2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D81D9CE2A426814A9054AC6C4C722ED5" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="64dce91d1c025dd40a65521324b61665">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="aa97a2c6-5066-49ad-90c0-e23f9da31bb2" xmlns:ns3="c319d79e-6821-4c2a-8db8-88a02643e5e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0b6c53cd2d86a7b8a56cde2aeea85a90" ns2:_="" ns3:_="">
     <xsd:import namespace="aa97a2c6-5066-49ad-90c0-e23f9da31bb2"/>
@@ -2715,7 +2715,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2724,18 +2724,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c319d79e-6821-4c2a-8db8-88a02643e5e3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="aa97a2c6-5066-49ad-90c0-e23f9da31bb2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A76C88C-3CD9-4DB8-BDE8-13FD5F7691CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c319d79e-6821-4c2a-8db8-88a02643e5e3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="aa97a2c6-5066-49ad-90c0-e23f9da31bb2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2294B864-0C2E-4EE7-BC4B-97F56F3E1E6F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2754,27 +2760,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F8ED70-8537-426E-A479-D2342A5FB5EB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A76C88C-3CD9-4DB8-BDE8-13FD5F7691CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c319d79e-6821-4c2a-8db8-88a02643e5e3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="aa97a2c6-5066-49ad-90c0-e23f9da31bb2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>